<commit_message>
Need larger sample size
</commit_message>
<xml_diff>
--- a/sample_text_with_emote.xlsx
+++ b/sample_text_with_emote.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/11d5e0df6c0ad6be/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4086DE8-3860-4F54-A2B2-0DD168C3C167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{F4086DE8-3860-4F54-A2B2-0DD168C3C167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AEA1ABA-E83A-443C-9808-5D5BA4AD6374}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" xr2:uid="{5532AA6A-2FDB-4791-B042-4D8AD181265C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5532AA6A-2FDB-4791-B042-4D8AD181265C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>message</t>
   </si>
   <si>
     <t>Hello my name is Shaun and I am in Computer Engineering and Management in McMaster and my partner Sachin Gupta is in software engineering also in Mac. We are looking for two hardworking backend demons that would be down to work on our project. Here is our linkedins: Shaun: https://www.linkedin.com/in/shaun-plassery-645381282/?originalSubdomain=ca Sachin: https://www.linkedin.com/in/sachin-ved-gupta/. Message me for more info if your down.</t>
-  </si>
-  <si>
-    <t>Hi everyone,
-I'm Shervin, an Engineering Science student at U of T (going into my second year), currently flying solo for Hack the 6ix. I have experience with embedded systems (Arduino, Raspberry Pi) and machine learning models from a previous hackathon.
-I'm eager to collaborate with people who are not only passionate about learning and building cool projects, but also chill and easy to get along with. If you're interested, shoot me a DM 👍</t>
   </si>
   <si>
     <t xml:space="preserve">Heyo,
@@ -91,36 +86,11 @@
 Github: https://github.com/MatthewFrieri</t>
   </si>
   <si>
-    <t>Yo I'm Nathan, I'm 16, and currently interning @Roboflow (YC 20) as a machine learning engineer. Mainly an MLE but have some experience backend too.
-looking for any team atp 😭
-CONNECT IWTH ME ON LINKEDIN PLEASE ALMOST REACHING 3.3K!!!
-linkedin:  https://www.linkedin.com/in/nathan-yan2008/</t>
-  </si>
-  <si>
     <t>wassup everyone I'm Rishabh and I'm a 3rd year CS major from UWaterloo. I have experience building embedded firmware, AI/ML models and full-stack applications. Currently, I'm a generative AI researcher at the National Research Council of Canada and Michigan State University. I want to build something dope that has real-world purpose, maybe something that sees the intersection of embedded systems and AI/ML? hmu if you want to work together. https://www.linkedin.com/in/rishabh2003sharma/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello everyone:D
-I'm Ryan and I'm going into my 5th year of CS at UBC! I'm a backend-focused dev starting my internship at Tesla for fall. I was one of the winners of UC Berkeley's CalHacks last year and aiming to grind next week:D Plz let me know if you're interested in forming a team (I don't wanna touch frontend 😭) Feel free to add me on LinkedIn: https://www.linkedin.com/in/ryan-mc-kim/ </t>
-  </si>
-  <si>
-    <t>hi! 👋 my name's tait berlette! i'm starting my first year at uoft for mechanical engineering in the fall! 
-i always really enjoy programming and programming, but i also love working with hardware (hence engineering lol) so i would be open to working on a hardware project if ppl are interested in that! i know c++/arduino, javascript/nodejs, java, and a bit of dart/flutter and python!
-at my last hackathon we built hardware for a telescope to be able to track space stations &amp; planets! https://taikai.network/hackbox/hackathons/hawkhacks/projects/clwdewjpl0dljuc0145ylzz1k/idea
-send me a dm if you are looking for someone to join your team!! my github: https://github.com/taitberlette</t>
   </si>
   <si>
     <t>Hi, I’m Mia, a third-year Math student at UWaterloo! I’m currently working as a full-stack developer, but I’m also interested in game development and computer vision. 
 Last year, I won first place at UWaterloo’s TechNova hackathon, and I’m hoping to continue that win streak here lol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi everyone, my name is Kersh. I'm currently a third year CS student at OTU with a Math minor. 
-Right now, I'm building a few side projects (emulator and a computer vision bot), but I have experience with full stack web development and embedded systems (mainly RPi and a bit of STM32). I really want to do something with ML and/or CV for this hackathon though to gain further knowledge and get ahead of co-op applications (as of rn, i know some pytorch and opencv).
-As for hackathon experience, I don't have that much, but in terms of what I've accomplished so far, my group won the Toronto chapter of last year's NASA Space Apps Challenge and ended up being a Global Finalist Honorable Mention.
-If y'all want to build a team or if you have room for one more, hmu on discord!
-I'm not looking for teammates anymore, since I have a team of 4. But, you can still connect with me on LinkedIn, GitHub and Discord(click on pfp)!
-LinkedIn: https://www.linkedin.com/in/kersharul/
-GitHub: https://github.com/Koops0 </t>
   </si>
   <si>
     <t xml:space="preserve">Hey everyone, I’m Andy. I’m a senior high school student, and my team and I are looking for two more members for Hack the 6ix. I have experience with Unity, Blender, backend, and mobile development, and my friend is a full-stack web developer. Additionally, we're both proficient in Python and SQL/NoSQL databases, and we have both been to plenty of hackathons. If you're interested, hit me up.
@@ -150,16 +120,6 @@
     <t>Hey, I’m Sydney! I’m a 4th year Cognitive Science major + Art &amp; Media minor at YorkU.  I don’t have too much coding experience, but I’m familiar with HTML, CSS, and Figma. I’m more experienced with graphic design and video editing, and I’d be more than happy to contribute my artistic skills to the team. This will be my first hackathon, and I’m excited to learn from everyone   DM me if you’d like to team up! 
 LinkedIn: https://www.linkedin.com/in/sydney-simota/
 Website: https://bysydneys.com/</t>
-  </si>
-  <si>
-    <t>Hey everyone! I'm An Vu, a new grad from April 2024 (and yes, really loving the job market right now 💀).
-I come from a cyber security background, specializing in .NET microservices, web, and backend dev with Python, Go, and C++. My friends and I just won the MLH prize at HawkHacks 2024!
-I'm teamed up with @Tait Berlette , a Mechanical Engineering student from UofT who just casually built a hardware for telescope to track space stations and planets at HawkHacks2024 🔥, and @Minh Vu , a UBC Stat student currently Data Analyst Intern at RBC Toronto who also happens to be an amazing artist 🌟.
-We'd love to have an ML enthusiast who's excited about doing a hardware project this time around. We're a super chill team and can't wait to meet everyone 😁.
-Check out our startup 🤟: https://klinkapp.com/ (yo, if you're a content creator, don't miss out on our platform)
-Portfolio: https://cyberanvu.co/
-LinkedIn: https://www.linkedin.com/in/an-vu-169817242/
-GitHub: https://github.com/anvu2002</t>
   </si>
   <si>
     <t>Hi, the name's Joudat
@@ -172,6 +132,45 @@
 LinkedIn - https://www.linkedin.com/in/joudat-haroon/
 GitHub - https://github.com/joutad
 Portfolio - http://joudat.netlify.app/</t>
+  </si>
+  <si>
+    <t>Yo I'm Nathan, I'm 16, and currently interning @Roboflow (YC 20) as a machine learning engineer. Mainly an MLE but have some experience backend too.
+looking for any team atp 
+CONNECT IWTH ME ON LINKEDIN PLEASE ALMOST REACHING 3.3K!!!
+linkedin:  https://www.linkedin.com/in/nathan-yan2008/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello everyone:D
+I'm Ryan and I'm going into my 5th year of CS at UBC! I'm a backend-focused dev starting my internship at Tesla for fall. I was one of the winners of UC Berkeley's CalHacks last year and aiming to grind next week:D Plz let me know if you're interested in forming a team (I don't wanna touch frontend ) Feel free to add me on LinkedIn: https://www.linkedin.com/in/ryan-mc-kim/ </t>
+  </si>
+  <si>
+    <t>hi!  my name's tait berlette! i'm starting my first year at uoft for mechanical engineering in the fall! 
+i always really enjoy programming and programming, but i also love working with hardware (hence engineering lol) so i would be open to working on a hardware project if ppl are interested in that! i know c++/arduino, javascript/nodejs, java, and a bit of dart/flutter and python!
+at my last hackathon we built hardware for a telescope to be able to track space stations &amp; planets! https://taikai.network/hackbox/hackathons/hawkhacks/projects/clwdewjpl0dljuc0145ylzz1k/idea
+send me a dm if you are looking for someone to join your team!! my github: https://github.com/taitberlette</t>
+  </si>
+  <si>
+    <t>Hey everyone! I'm An Vu, a new grad from April 2024 (and yes, really loving the job market right now ).
+I come from a cyber security background, specializing in .NET microservices, web, and backend dev with Python, Go, and C++. My friends and I just won the MLH prize at HawkHacks 2024!
+I'm teamed up with @Tait Berlette , a Mechanical Engineering student from UofT who just casually built a hardware for telescope to track space stations and planets at HawkHacks2024 , and @Minh Vu , a UBC Stat student currently Data Analyst Intern at RBC Toronto who also happens to be an amazing artist .
+We'd love to have an ML enthusiast who's excited about doing a hardware project this time around. We're a super chill team and can't wait to meet everyone .
+Check out our startup : https://klinkapp.com/ (yo, if you're a content creator, don't miss out on our platform)
+Portfolio: https://cyberanvu.co/
+LinkedIn: https://www.linkedin.com/in/an-vu-169817242/
+GitHub: https://github.com/anvu2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi everyone,
+I'm Shervin, an Engineering Science student at U of T (going into my second year), currently flying solo for Hack the 6ix. I have experience with embedded systems (Arduino, Raspberry Pi) and machine learning models from a previous hackathon.
+I'm eager to collaborate with people who are not only passionate about learning and building cool projects, but also chill and easy to get along with. If you're interested, shoot me a DM </t>
+  </si>
+  <si>
+    <t>Hi everyone, my name is Kersh. I'm currently a third year CS student at OTU with a Math minor. 
+Right now, I'm building a few side projects (emulator and a computer vision bot), but I have experience with full stack web development and embedded systems (mainly RPi and a bit of STM32). I really want to do something with ML and/or CV for this hackathon though to gain further knowledge and get ahead of co-op applications (as of rn, i know some pytorch and opencv).
+As for hackathon experience, I don't have that much, but in terms of what I've accomplished so far, my group won the Toronto chapter of last year's NASA Space Apps Challenge and ended up being a Global Finalist Honorable Mention.
+If y'all want to build a team or if you have room for one more, hmu on discord!
+I'm not looking for teammates anymore, since I have a team of 4. But, you can still connect with me on LinkedIn, GitHub and Discord(click on pfp)!
+LinkedIn: https://www.linkedin.com/in/kersharul/</t>
   </si>
 </sst>
 </file>
@@ -546,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CAC3F2-1712-4DF5-AB62-EDBA859EE720}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,106 +566,134 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="13" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1"/>
+    </row>
+    <row r="24" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>